<commit_message>
updates + developed a top_5_name_mvp_ppg chart via matplotlib
</commit_message>
<xml_diff>
--- a/top_10_nba_mvp_ppg_df.xlsx
+++ b/top_10_nba_mvp_ppg_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>season</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>team</t>
-  </si>
-  <si>
-    <t>first</t>
   </si>
   <si>
     <t>pts_per_game</t>
@@ -434,13 +431,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,237 +456,204 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1960</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
       <c r="D2">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2">
-        <v>49</v>
-      </c>
-      <c r="G2">
         <v>37.6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1988</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3">
-        <v>47</v>
-      </c>
-      <c r="G3">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1972</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4">
-        <v>81</v>
-      </c>
-      <c r="G4">
         <v>34.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1975</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5">
-        <v>81</v>
-      </c>
-      <c r="G5">
         <v>34.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>1966</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
       </c>
       <c r="D6">
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6">
-        <v>48</v>
-      </c>
-      <c r="G6">
         <v>33.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2023</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7">
-        <v>73</v>
-      </c>
-      <c r="G7">
         <v>33.1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>2014</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8">
-        <v>119</v>
-      </c>
-      <c r="G8">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>1971</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9">
-        <v>133</v>
-      </c>
-      <c r="G9">
         <v>31.7</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>2017</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10">
-        <v>69</v>
-      </c>
-      <c r="G10">
         <v>31.6</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>1991</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11">
-        <v>77</v>
-      </c>
-      <c r="G11">
         <v>31.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
converting season values to string format and updating them accordingly
</commit_message>
<xml_diff>
--- a/top_10_nba_mvp_ppg_df.xlsx
+++ b/top_10_nba_mvp_ppg_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>season</t>
   </si>
@@ -32,6 +32,36 @@
   </si>
   <si>
     <t>pts_per_game</t>
+  </si>
+  <si>
+    <t>1960</t>
+  </si>
+  <si>
+    <t>1988</t>
+  </si>
+  <si>
+    <t>1972</t>
+  </si>
+  <si>
+    <t>1975</t>
+  </si>
+  <si>
+    <t>1966</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>1971</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>1991</t>
   </si>
   <si>
     <t>nba mvp</t>
@@ -458,200 +488,200 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2">
-        <v>1960</v>
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>37.6</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3">
-        <v>1988</v>
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F3">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4">
-        <v>1972</v>
+      <c r="A4" t="s">
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F4">
         <v>34.8</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5">
-        <v>1975</v>
+      <c r="A5" t="s">
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F5">
         <v>34.5</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6">
-        <v>1966</v>
+      <c r="A6" t="s">
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F6">
         <v>33.5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7">
-        <v>2023</v>
+      <c r="A7" t="s">
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F7">
         <v>33.1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8">
-        <v>2014</v>
+      <c r="A8" t="s">
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D8">
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F8">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9">
-        <v>1971</v>
+      <c r="A9" t="s">
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F9">
         <v>31.7</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10">
-        <v>2017</v>
+      <c r="A10" t="s">
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F10">
         <v>31.6</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11">
-        <v>1991</v>
+      <c r="A11" t="s">
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D11">
         <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F11">
         <v>31.5</v>

</xml_diff>

<commit_message>
various additions/modifications to all dataframes
</commit_message>
<xml_diff>
--- a/top_10_nba_mvp_ppg_df.xlsx
+++ b/top_10_nba_mvp_ppg_df.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
-  <si>
-    <t>season</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+  <si>
+    <t>year</t>
   </si>
   <si>
     <t>award</t>
@@ -31,7 +31,13 @@
     <t>team</t>
   </si>
   <si>
+    <t>pf_per_game</t>
+  </si>
+  <si>
     <t>pts_per_game</t>
+  </si>
+  <si>
+    <t>season_y</t>
   </si>
   <si>
     <t>1960</t>
@@ -461,13 +467,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,205 +492,271 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F2">
+        <v>2.1</v>
+      </c>
+      <c r="G2">
         <v>37.6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F3">
+        <v>3.3</v>
+      </c>
+      <c r="G3">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4">
+        <v>2.9</v>
+      </c>
+      <c r="G4">
         <v>34.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F5">
+        <v>3.4</v>
+      </c>
+      <c r="G5">
         <v>34.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F6">
+        <v>2.2</v>
+      </c>
+      <c r="G6">
         <v>33.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F7">
+        <v>3.1</v>
+      </c>
+      <c r="G7">
         <v>33.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F8">
+        <v>2.1</v>
+      </c>
+      <c r="G8">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F9">
+        <v>3.2</v>
+      </c>
+      <c r="G9">
         <v>31.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F10">
+        <v>2.3</v>
+      </c>
+      <c r="G10">
         <v>31.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F11">
+        <v>2.8</v>
+      </c>
+      <c r="G11">
         <v>31.5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates in double_double_avg and triple_double_avg columns to player_per_game_df
</commit_message>
<xml_diff>
--- a/top_10_nba_mvp_ppg_df.xlsx
+++ b/top_10_nba_mvp_ppg_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
   <si>
     <t>year</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>double_double_avg</t>
+  </si>
+  <si>
+    <t>triple_double_avg</t>
   </si>
   <si>
     <t>1960</t>
@@ -506,13 +509,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,22 +543,25 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F2">
         <v>2.1</v>
@@ -564,27 +570,30 @@
         <v>37.6</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3">
         <v>3.3</v>
@@ -593,27 +602,30 @@
         <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>45</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4">
         <v>2.9</v>
@@ -622,27 +634,30 @@
         <v>34.8</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>44</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F5">
         <v>3.4</v>
@@ -651,27 +666,30 @@
         <v>34.5</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6">
         <v>2.2</v>
@@ -680,27 +698,30 @@
         <v>33.5</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F7">
         <v>3.1</v>
@@ -709,27 +730,30 @@
         <v>33.1</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>44</v>
+      </c>
+      <c r="J7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8">
         <v>2.1</v>
@@ -738,27 +762,30 @@
         <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>45</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F9">
         <v>3.2</v>
@@ -767,27 +794,30 @@
         <v>31.7</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>44</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10">
         <v>2.3</v>
@@ -796,27 +826,30 @@
         <v>31.6</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>44</v>
+      </c>
+      <c r="J10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11">
         <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F11">
         <v>2.8</v>
@@ -825,10 +858,13 @@
         <v>31.5</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I11" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="J11" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>